<commit_message>
Changed variant count column for venn diagram.
</commit_message>
<xml_diff>
--- a/Results/Data_Venn.xlsx
+++ b/Results/Data_Venn.xlsx
@@ -19,7 +19,7 @@
     <t>PATIENT-ID</t>
   </si>
   <si>
-    <t>TUMOR-DETECTED-PVALUE</t>
+    <t>COUNT-VARIANTS-DETECTED</t>
   </si>
   <si>
     <t>S100</t>
@@ -558,7 +558,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>9.999999999999999E-21</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>0.795</v>
@@ -572,7 +572,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>9.999999999999999E-21</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>0.051</v>
@@ -586,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>9.999999999999999E-21</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>3.12</v>
@@ -600,7 +600,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>9.999999999999999E-21</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>0.535</v>
@@ -614,7 +614,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>9.999999999999999E-21</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>0.333</v>
@@ -628,7 +628,7 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>9.999999999999999E-21</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>0.164</v>
@@ -642,7 +642,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>9.999999999999999E-21</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>3.18</v>
@@ -656,7 +656,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>9.999999999999999E-21</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>0.123</v>
@@ -670,7 +670,7 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>9.999999999999999E-21</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>0.873</v>
@@ -684,7 +684,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>9.999999999999999E-21</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>2.66</v>
@@ -698,7 +698,7 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>9.999999999999999E-21</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>0.83</v>
@@ -712,7 +712,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>9.999999999999999E-21</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>13.48</v>
@@ -726,7 +726,7 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>9.999999999999999E-21</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>1.24</v>
@@ -740,7 +740,7 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>9.999999999999999E-21</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>0.067</v>
@@ -754,7 +754,7 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>6.515847031540595E-11</v>
+        <v>8</v>
       </c>
       <c r="C16">
         <v>0.07000000000000001</v>
@@ -768,7 +768,7 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>9.999999999999999E-21</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>0.358</v>
@@ -782,7 +782,7 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>9.999999999999999E-21</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>0.379</v>
@@ -796,7 +796,7 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>9.999999999999999E-21</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>0.3</v>
@@ -810,7 +810,7 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>9.999999999999999E-21</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>3.9</v>
@@ -824,7 +824,7 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>9.999999999999999E-21</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>0.126</v>
@@ -838,7 +838,7 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>0.9996615968367696</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>0.092</v>
@@ -852,7 +852,7 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>9.999999999999999E-21</v>
+        <v>16</v>
       </c>
       <c r="C23">
         <v>0.098</v>
@@ -866,7 +866,7 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>9.999999999999999E-21</v>
+        <v>21</v>
       </c>
       <c r="C24">
         <v>0.466</v>
@@ -880,7 +880,7 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>9.999999999999999E-21</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>0.245</v>
@@ -894,7 +894,7 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>9.999999999999999E-21</v>
+        <v>21</v>
       </c>
       <c r="C26">
         <v>4.13</v>
@@ -908,7 +908,7 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>0.0187161719154362</v>
+        <v>5</v>
       </c>
       <c r="C27">
         <v>0.032</v>
@@ -922,7 +922,7 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>0.0530999999999999</v>
+        <v>4</v>
       </c>
       <c r="C28">
         <v>0.053</v>
@@ -936,7 +936,7 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
         <v>0.061</v>
@@ -950,7 +950,7 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>9.999999999999999E-21</v>
+        <v>27</v>
       </c>
       <c r="C30">
         <v>0.052</v>
@@ -964,7 +964,7 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>1.603782285138741E-10</v>
+        <v>4</v>
       </c>
       <c r="C31">
         <v>0.048</v>
@@ -978,7 +978,7 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>9.999999999999999E-21</v>
+        <v>19</v>
       </c>
       <c r="C32">
         <v>0.039</v>
@@ -992,7 +992,7 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>0.2164443564676841</v>
+        <v>3</v>
       </c>
       <c r="C33">
         <v>0.033</v>
@@ -1006,7 +1006,7 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>4.066628165885049E-09</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>0.5629999999999999</v>
@@ -1020,7 +1020,7 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>1.810443253132819E-05</v>
+        <v>3</v>
       </c>
       <c r="C35">
         <v>0.079</v>
@@ -1034,7 +1034,7 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <v>0.06</v>
@@ -1048,7 +1048,7 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>0.9862146604273798</v>
+        <v>2</v>
       </c>
       <c r="C37">
         <v>0.03</v>
@@ -1062,7 +1062,7 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>9.999999999999999E-21</v>
+        <v>27</v>
       </c>
       <c r="C38">
         <v>0.204</v>
@@ -1076,7 +1076,7 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>9.999999999999999E-21</v>
+        <v>21</v>
       </c>
       <c r="C39">
         <v>0.025</v>
@@ -1090,7 +1090,7 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>9.999999999999999E-21</v>
+        <v>5</v>
       </c>
       <c r="C40">
         <v>0.657</v>
@@ -1104,7 +1104,7 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>9.999999999999999E-21</v>
+        <v>24</v>
       </c>
       <c r="C41">
         <v>0.081</v>
@@ -1118,7 +1118,7 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>9.999999999999999E-21</v>
+        <v>14</v>
       </c>
       <c r="C42">
         <v>0.378</v>
@@ -1132,7 +1132,7 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>9.999999999999999E-21</v>
+        <v>8</v>
       </c>
       <c r="C43">
         <v>0.098</v>
@@ -1146,7 +1146,7 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>9.999999999999999E-21</v>
+        <v>26</v>
       </c>
       <c r="C44">
         <v>0.08699999999999999</v>
@@ -1160,7 +1160,7 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>9.999999999999999E-21</v>
+        <v>4</v>
       </c>
       <c r="C45">
         <v>0.082</v>
@@ -1174,7 +1174,7 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>9.999999999999999E-21</v>
+        <v>22</v>
       </c>
       <c r="C46">
         <v>0.984</v>
@@ -1188,7 +1188,7 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>9.999999999999999E-21</v>
+        <v>9</v>
       </c>
       <c r="C47">
         <v>1.64</v>
@@ -1202,7 +1202,7 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>9.999999999999999E-21</v>
+        <v>30</v>
       </c>
       <c r="C48">
         <v>0.273</v>
@@ -1216,7 +1216,7 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>9.966156270240726E-07</v>
+        <v>3</v>
       </c>
       <c r="C49">
         <v>0.063</v>
@@ -1230,7 +1230,7 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>9.999999999999999E-21</v>
+        <v>3</v>
       </c>
       <c r="C50">
         <v>0.244</v>
@@ -1244,7 +1244,7 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>9.999999999999999E-21</v>
+        <v>29</v>
       </c>
       <c r="C51">
         <v>0.138</v>

</xml_diff>